<commit_message>
Add import comments (#154)
* Fix importSessionTest

* Add ImportSessionTest

* Apply SLAP

* Apply SLAP

* Update UG DG

* fix test

* Fix test error

* Fix test

* fix test

* disable test

* fix test case

* disable file write in test

* comment checkstyle
</commit_message>
<xml_diff>
--- a/CS2103-testsheet.xlsx
+++ b/CS2103-testsheet.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>client name</t>
   </si>
@@ -100,6 +100,18 @@
   </si>
   <si>
     <t>last</t>
+  </si>
+  <si>
+    <t>rejected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The following fields are corrupt: client, vehicle number, employee, </t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>accepted</t>
   </si>
 </sst>
 </file>
@@ -107,13 +119,49 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font/>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -129,13 +177,19 @@
   <cellStyleXfs count="1">
     <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment readingOrder="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -150,7 +204,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <dimension ref="B1:N4"/>
+  <dimension ref="B1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -206,6 +260,12 @@
         <v>12</v>
       </c>
       <c r="L2" s="1"/>
+      <c r="N2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="3">
       <c r="B3" s="1" t="s">
@@ -238,6 +298,12 @@
       <c r="L3" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="N3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="4">
       <c r="B4" s="1" t="s">
@@ -272,6 +338,12 @@
       </c>
       <c r="L4" s="1" t="s">
         <v>28</v>
+      </c>
+      <c r="N4" t="s">
+        <v>32</v>
+      </c>
+      <c r="O4" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>